<commit_message>
Implemented random forces and thus completed rotation
</commit_message>
<xml_diff>
--- a/Pressure Testing.xlsx
+++ b/Pressure Testing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="P Test - N_WATER" sheetId="2" r:id="rId1"/>
@@ -739,7 +739,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -821,7 +820,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1946,7 +1944,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2406,7 +2403,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2488,7 +2484,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8038,7 +8033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -9395,8 +9390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fiddled with LE BC, changed EoM to follow SLLOD (no diff for noshear), and added automator
</commit_message>
<xml_diff>
--- a/Pressure Testing.xlsx
+++ b/Pressure Testing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="P Test - N_WATER" sheetId="2" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>alpha</t>
   </si>
   <si>
-    <t>p_reduce</t>
-  </si>
-  <si>
     <t>BOX_SIZE</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>Stdev</t>
+  </si>
+  <si>
+    <t>p - rho</t>
   </si>
 </sst>
 </file>
@@ -739,6 +739,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -820,6 +821,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1944,6 +1946,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2403,6 +2406,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2484,6 +2488,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2866,7 +2871,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.6580941946837696E-2"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.89653016109583572"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2906,6 +2921,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.8574590676857102E-2"/>
+                  <c:y val="0.14158136482939632"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -8033,8 +8098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8073,7 +8138,7 @@
         <v>22</v>
       </c>
       <c r="M1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="N1" t="s">
         <v>23</v>
@@ -8957,7 +9022,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8974,7 +9039,7 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>19</v>
@@ -9364,7 +9429,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -9390,8 +9455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9408,7 +9473,7 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
@@ -9423,16 +9488,16 @@
         <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
         <v>28</v>
-      </c>
-      <c r="M1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>